<commit_message>
mise a jour du controle des colonnes avec messages dynamiques
</commit_message>
<xml_diff>
--- a/Accès aux outils - Profils types et outils.xlsx
+++ b/Accès aux outils - Profils types et outils.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="13" documentId="8_{F6824792-E74A-464D-8801-638C225AF9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94BBFC9D-0407-4D03-A8F1-736CF5C748A1}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="20570" yWindow="3750" windowWidth="14450" windowHeight="8210" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16690" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des profils" sheetId="3" r:id="rId1"/>
@@ -2850,21 +2850,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Valid_x00e9_r_x00e9_f_x00e9_rent xmlns="a497ef4b-d577-435f-96f3-059014e6626f">Non</Valid_x00e9_r_x00e9_f_x00e9_rent>
-    <TaxCatchAll xmlns="1b664402-d62c-4bf8-8d02-c93b84fb4f47" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a497ef4b-d577-435f-96f3-059014e6626f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_Flow_SignoffStatus xmlns="a497ef4b-d577-435f-96f3-059014e6626f" xsi:nil="true"/>
-    <D_x00e9_tail xmlns="a497ef4b-d577-435f-96f3-059014e6626f" xsi:nil="true"/>
-    <Emplacement xmlns="a497ef4b-d577-435f-96f3-059014e6626f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010060787147F1F0B5439FB4A9998F7C2B0E" ma:contentTypeVersion="30" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="7c3b68090481f80331bb85e91e4b8e30">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a497ef4b-d577-435f-96f3-059014e6626f" xmlns:ns3="1b664402-d62c-4bf8-8d02-c93b84fb4f47" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="686db46c1752b9b2ebb4c6ca041c1c82" ns2:_="" ns3:_="">
     <xsd:import namespace="a497ef4b-d577-435f-96f3-059014e6626f"/>
@@ -3189,6 +3174,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Valid_x00e9_r_x00e9_f_x00e9_rent xmlns="a497ef4b-d577-435f-96f3-059014e6626f">Non</Valid_x00e9_r_x00e9_f_x00e9_rent>
+    <TaxCatchAll xmlns="1b664402-d62c-4bf8-8d02-c93b84fb4f47" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a497ef4b-d577-435f-96f3-059014e6626f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_Flow_SignoffStatus xmlns="a497ef4b-d577-435f-96f3-059014e6626f" xsi:nil="true"/>
+    <D_x00e9_tail xmlns="a497ef4b-d577-435f-96f3-059014e6626f" xsi:nil="true"/>
+    <Emplacement xmlns="a497ef4b-d577-435f-96f3-059014e6626f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3199,17 +3199,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{461ED897-2A71-4D26-934C-560A060C55A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a497ef4b-d577-435f-96f3-059014e6626f"/>
-    <ds:schemaRef ds:uri="1b664402-d62c-4bf8-8d02-c93b84fb4f47"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D6BB09E-C2F5-4DE9-BA97-BA134CA64151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3228,6 +3217,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{461ED897-2A71-4D26-934C-560A060C55A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a497ef4b-d577-435f-96f3-059014e6626f"/>
+    <ds:schemaRef ds:uri="1b664402-d62c-4bf8-8d02-c93b84fb4f47"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{541676A7-2F1E-42F4-8588-60C2ED865A0E}">
   <ds:schemaRefs>

</xml_diff>